<commit_message>
update and modified commit
</commit_message>
<xml_diff>
--- a/src/test/resources/excel/DataTest.xlsx
+++ b/src/test/resources/excel/DataTest.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProject\Java\MyProject\DataDrivenFramework\src\test\resources\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\CodeProject\Java\MyProject\SeleniumWebAutomation\src\test\resources\excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21659755-F1FA-448E-B714-F5536E36025D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DF22D2-3417-4B8E-8782-D7D1967A1E64}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1155" yWindow="3465" windowWidth="26955" windowHeight="11310" activeTab="2" xr2:uid="{575F2EE9-8424-4FBD-A84E-5558AA6916D6}"/>
+    <workbookView xWindow="3495" yWindow="3525" windowWidth="21600" windowHeight="11295" xr2:uid="{575F2EE9-8424-4FBD-A84E-5558AA6916D6}"/>
   </bookViews>
   <sheets>
-    <sheet name="TestSuite" sheetId="3" r:id="rId1"/>
+    <sheet name="TestSuite" sheetId="4" r:id="rId1"/>
     <sheet name="AddCustomerTest" sheetId="1" r:id="rId2"/>
     <sheet name="OpenAccountTest" sheetId="2" r:id="rId3"/>
   </sheets>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="59">
   <si>
     <t>FirstName</t>
   </si>
@@ -52,65 +52,176 @@
     <t>TCID</t>
   </si>
   <si>
-    <t>BankManagerLoginTest</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
+    <t>RunMode</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Currency</t>
+  </si>
+  <si>
+    <t>Harry Potter</t>
+  </si>
+  <si>
+    <t>Pound</t>
+  </si>
+  <si>
+    <t>TestCaseName</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>Charita</t>
+  </si>
+  <si>
+    <t>Mathivon</t>
+  </si>
+  <si>
+    <t>Elias</t>
+  </si>
+  <si>
+    <t>Jossum</t>
+  </si>
+  <si>
+    <t>BM-001</t>
+  </si>
+  <si>
+    <t>BM-002</t>
+  </si>
+  <si>
+    <t>BM-003</t>
+  </si>
+  <si>
+    <t>TS-001</t>
+  </si>
+  <si>
+    <t>TS-002</t>
+  </si>
+  <si>
+    <t>BankManagerLogInTest</t>
+  </si>
+  <si>
     <t>AddCustomerTest</t>
   </si>
   <si>
     <t>OpenAccountTest</t>
   </si>
   <si>
-    <t>RunMode</t>
-  </si>
-  <si>
-    <t>Customer</t>
-  </si>
-  <si>
-    <t>Currency</t>
-  </si>
-  <si>
-    <t>Harry Potter</t>
-  </si>
-  <si>
-    <t>Pound</t>
-  </si>
-  <si>
-    <t>TestCaseName</t>
-  </si>
-  <si>
-    <t>TC-001</t>
-  </si>
-  <si>
-    <t>TC-002</t>
-  </si>
-  <si>
-    <t>TC-003</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>Charita</t>
-  </si>
-  <si>
-    <t>Mathivon</t>
-  </si>
-  <si>
-    <t>Elias</t>
-  </si>
-  <si>
-    <t>Jossum</t>
+    <t>CS-001</t>
+  </si>
+  <si>
+    <t>CustomerLoginTest</t>
+  </si>
+  <si>
+    <t>CS-002</t>
+  </si>
+  <si>
+    <t>CustomerProfilePageTest</t>
+  </si>
+  <si>
+    <t>CS-003</t>
+  </si>
+  <si>
+    <t>CountCustomerAccountTest</t>
+  </si>
+  <si>
+    <t>CS-004</t>
+  </si>
+  <si>
+    <t>CheckCustomerCurrentBalanceTest</t>
+  </si>
+  <si>
+    <t>CS-005</t>
+  </si>
+  <si>
+    <t>CheckCustomerCurrencyTest</t>
+  </si>
+  <si>
+    <t>CS-006</t>
+  </si>
+  <si>
+    <t>CustomerAccountCheckTest</t>
+  </si>
+  <si>
+    <t>CS-007</t>
+  </si>
+  <si>
+    <t>CustomerLogoutTest</t>
+  </si>
+  <si>
+    <t>CustomerDepositTest</t>
+  </si>
+  <si>
+    <t>TS-003</t>
+  </si>
+  <si>
+    <t>CustomerPageListTest</t>
+  </si>
+  <si>
+    <t>BM-004</t>
+  </si>
+  <si>
+    <t>DeleteFunctionalityTest</t>
+  </si>
+  <si>
+    <t>BM-005</t>
+  </si>
+  <si>
+    <t>BM-006</t>
+  </si>
+  <si>
+    <t>CustomerHeaderListTest</t>
+  </si>
+  <si>
+    <t>DeleteButtonPresentTest</t>
+  </si>
+  <si>
+    <t>DeleteSpecificDataTest</t>
+  </si>
+  <si>
+    <t>BM-007</t>
+  </si>
+  <si>
+    <t>BM-008</t>
+  </si>
+  <si>
+    <t>SearchCustomerValidDataTest</t>
+  </si>
+  <si>
+    <t>BM-009</t>
+  </si>
+  <si>
+    <t>SearchCustomerInvalidDataTest</t>
+  </si>
+  <si>
+    <t>VerifyCustomerLoginTest</t>
+  </si>
+  <si>
+    <t>CS-008</t>
+  </si>
+  <si>
+    <t>CheckBalanceTest</t>
+  </si>
+  <si>
+    <t>WithdrawTest</t>
+  </si>
+  <si>
+    <t>TS-004</t>
+  </si>
+  <si>
+    <t>CheckTransactionHistoryTest</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,8 +237,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -137,6 +254,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -168,7 +291,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -178,6 +301,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -511,61 +638,292 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EED8B81-DE94-425E-8B46-7FC321A1E050}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C420A538-CC19-4CC0-9147-F6CC70534995}">
+  <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>4</v>
+        <v>21</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>6</v>
+        <v>17</v>
+      </c>
+      <c r="B3" s="5" t="s">
+        <v>22</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>7</v>
+        <v>18</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>23</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>5</v>
-      </c>
+        <v>4</v>
+      </c>
+      <c r="D4" s="6"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" s="6"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D6" s="6"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="6"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="6"/>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D9" s="6"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B10" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D10" s="6"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D11" s="6"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D12" s="6"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D13" s="6"/>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D14" s="6"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D15" s="6"/>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D16" s="6"/>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D17" s="6"/>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="6"/>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D19" s="6"/>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D20" s="6"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D21" s="6"/>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D22" s="6"/>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="D23" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -598,35 +956,35 @@
         <v>2</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C2" s="2">
         <v>41351</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="C3" s="2">
         <v>20022</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>
@@ -638,7 +996,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A842AC83-D7C3-49A1-A684-AF0612E5A9CA}">
   <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G18" sqref="G18"/>
     </sheetView>
   </sheetViews>
@@ -649,24 +1007,24 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>